<commit_message>
Newest records backup, some fractal research changes (no idea what)
</commit_message>
<xml_diff>
--- a/Research/Fractal.xlsx
+++ b/Research/Fractal.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Health" sheetId="2" r:id="rId1"/>
     <sheet name="Taul1" sheetId="3" r:id="rId2"/>
+    <sheet name="Health data" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Big</t>
   </si>
@@ -89,6 +90,15 @@
   <si>
     <t>base</t>
   </si>
+  <si>
+    <t>Dulfy</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t>Grawl</t>
+  </si>
 </sst>
 </file>
 
@@ -128,12 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -149,6 +160,2945 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Veteran</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Health data'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Health data'!$B$3:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0418410041841004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1220679599340688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5277133257258779</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Dulfy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fi-FI"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Health data'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Health data'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>315480</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>328680</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>353990</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>481963</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>843506</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2016847232"/>
+        <c:axId val="2016858656"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2016847232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2016858656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2016858656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2016847232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Health data'!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Grawl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fi-FI"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Health data'!$A$12:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Health data'!$C$12:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>744360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>782760</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1028441</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1442645</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1661231</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2178658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2005907664"/>
+        <c:axId val="2005902224"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2005907664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005902224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2005902224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005907664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Testi</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.25128674540682416"/>
+                  <c:y val="7.2907553222513859E-5"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fi-FI"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.36800831146106738"/>
+                  <c:y val="-1.0189559638378537E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fi-FI"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Health data'!$A$21:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Health data'!$B$21:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0418410041841004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0515879413187168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1220679599340688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3816446343167286</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5277133257258779</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.938101187597399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2317574829383631</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6737225814631671</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9268875275404374</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2142099408"/>
+        <c:axId val="2142117360"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="2142099408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2142117360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2142117360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2142099408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Kaavio 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Kaavio 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Kaavio 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,7 +3366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -4028,4 +6978,454 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1">
+        <f>C2*$O$22</f>
+        <v>1947.9944865387715</v>
+      </c>
+      <c r="F1">
+        <f>C2*$O$23</f>
+        <v>157.21021602450426</v>
+      </c>
+      <c r="G1">
+        <f>C2*$O$24</f>
+        <v>-5.7479442205384492</v>
+      </c>
+      <c r="H1">
+        <f>C2*$O$25</f>
+        <v>0.13549754957278734</v>
+      </c>
+      <c r="I1">
+        <f>C2*$O$26</f>
+        <v>-8.4765436079316464E-4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>15 *(5922+10*ROUND(1374*1.1,0))</f>
+        <v>315480</v>
+      </c>
+      <c r="N2">
+        <f>18450/C2</f>
+        <v>5.8482312666413086E-2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2">
+        <v>29880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>C3/$C$2</f>
+        <v>1.0418410041841004</v>
+      </c>
+      <c r="C3">
+        <v>328680</v>
+      </c>
+      <c r="D3">
+        <f>$C$2+A3*$E$1 + A3*A3*$F$1+A3*A3*A3*$G$1 +A3*A3*A3*A3*$H$1+A3*A3*A3*A3*A3*$I$1</f>
+        <v>317579.59140823787</v>
+      </c>
+      <c r="N3">
+        <f>108945/C2</f>
+        <v>0.34533092430581969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <f>C4/$C$2</f>
+        <v>1.1220679599340688</v>
+      </c>
+      <c r="C4">
+        <v>353990</v>
+      </c>
+      <c r="N4">
+        <f>213712/C2</f>
+        <v>0.67741853683276276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <f>C5/$C$2</f>
+        <v>1.5277133257258779</v>
+      </c>
+      <c r="C5">
+        <v>481963</v>
+      </c>
+      <c r="N5">
+        <f>191746/C2</f>
+        <v>0.60779130214276655</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <f>C6/$C$2</f>
+        <v>2.6737225814631671</v>
+      </c>
+      <c r="C6">
+        <v>843506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="N7">
+        <f>1683.9/C2</f>
+        <v>5.3375808292126289E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="N8">
+        <f>1757/C2</f>
+        <v>5.5692912387473054E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="N9">
+        <f>25471/C2</f>
+        <v>8.0737289210092558E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="N10">
+        <f>76593/C2</f>
+        <v>0.24278242677824269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <f>C12*$O$22</f>
+        <v>4596.2</v>
+      </c>
+      <c r="F11">
+        <f>C12*$O$23</f>
+        <v>370.92999999999995</v>
+      </c>
+      <c r="G11">
+        <f>C12*$O$24</f>
+        <v>-13.561999999999999</v>
+      </c>
+      <c r="H11">
+        <f>C12*$O$25</f>
+        <v>0.31969999999999998</v>
+      </c>
+      <c r="I11">
+        <f>C12*$O$26</f>
+        <v>-2E-3</v>
+      </c>
+      <c r="N11">
+        <f>264491/C2</f>
+        <v>0.83837644224673513</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>30 *(5922+10*ROUND(1374*1.375,0))</f>
+        <v>744360</v>
+      </c>
+      <c r="F12">
+        <f>$C12*F21</f>
+        <v>752399.08799999999</v>
+      </c>
+      <c r="G12">
+        <f>$C12*G21</f>
+        <v>6848.1120000000001</v>
+      </c>
+      <c r="H12">
+        <f>$C12*H21</f>
+        <v>22.3308</v>
+      </c>
+      <c r="I12">
+        <f>$C12*I21</f>
+        <v>3.7218000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f>C13/$C$12</f>
+        <v>1.0515879413187168</v>
+      </c>
+      <c r="C13">
+        <v>782760</v>
+      </c>
+      <c r="D13">
+        <f>$C$12+A13*$E$11 + A13*A13*$F$11+A13*A13*A13*$G$11 +A13*A13*A13*A13*$H$11+A13*A13*A13*A13*A13*$I$11</f>
+        <v>782760.06719999993</v>
+      </c>
+      <c r="E13">
+        <f>F$12+A13*G$12+A13+ A13*A13*H$12+A13*A13*A13*I$12</f>
+        <v>795101.57759999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <f>C14/$C$12</f>
+        <v>1.3816446343167286</v>
+      </c>
+      <c r="C14">
+        <v>1028441</v>
+      </c>
+      <c r="D14">
+        <f>$C$12+A14*$E$11 + A14*A14*$F$11+A14*A14*A14*$G$11 +A14*A14*A14*A14*$H$11+A14*A14*A14*A14*A14*$I$11</f>
+        <v>1028234.4831999999</v>
+      </c>
+      <c r="E14">
+        <f>F$12+A14*G$12+A14+ A14*A14*H$12+A14*A14*A14*I$12</f>
+        <v>1043382.5247999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <f>C15/$C$12</f>
+        <v>1.938101187597399</v>
+      </c>
+      <c r="C15">
+        <v>1442645</v>
+      </c>
+      <c r="D15">
+        <f>$C$12+A15*$E$11 + A15*A15*$F$11+A15*A15*A15*$G$11 +A15*A15*A15*A15*$H$11+A15*A15*A15*A15*A15*$I$11</f>
+        <v>1440118.9791999997</v>
+      </c>
+      <c r="E15">
+        <f>F$12+A15*G$12+A15+ A15*A15*H$12+A15*A15*A15*I$12</f>
+        <v>1476975.3376000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <f>C16/$C$12</f>
+        <v>2.2317574829383631</v>
+      </c>
+      <c r="C16">
+        <v>1661231</v>
+      </c>
+      <c r="D16">
+        <f>$C$12+A16*$E$11 + A16*A16*$F$11+A16*A16*A16*$G$11 +A16*A16*A16*A16*$H$11+A16*A16*A16*A16*A16*$I$11</f>
+        <v>1656546.9952</v>
+      </c>
+      <c r="E16">
+        <f>F$12+A16*G$12+A16+ A16*A16*H$12+A16*A16*A16*I$12</f>
+        <v>1692250.2496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <f>C17/$C$12</f>
+        <v>2.9268875275404374</v>
+      </c>
+      <c r="C17">
+        <v>2178658</v>
+      </c>
+      <c r="D17">
+        <f>$C$12+A17*$E$11 + A17*A17*$F$11+A17*A17*A17*$G$11 +A17*A17*A17*A17*$H$11+A17*A17*A17*A17*A17*$I$11</f>
+        <v>2166352.9016999993</v>
+      </c>
+      <c r="E17">
+        <f>F$12+A17*G$12+A17+ A17*A17*H$12+A17*A17*A17*I$12</f>
+        <v>2203149.0137999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1.0107999999999999</v>
+      </c>
+      <c r="G21">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="Q21">
+        <v>741705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1.0418410041841004</v>
+      </c>
+      <c r="N22">
+        <v>4596.2</v>
+      </c>
+      <c r="O22">
+        <f>N22/$C$12</f>
+        <v>6.174700413778279E-3</v>
+      </c>
+      <c r="Q22">
+        <v>7623.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1.0515879413187168</v>
+      </c>
+      <c r="N23">
+        <v>370.93</v>
+      </c>
+      <c r="O23">
+        <f>N23/$C$12</f>
+        <v>4.9832070503519799E-4</v>
+      </c>
+      <c r="Q23">
+        <v>-32.813000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>1.1220679599340688</v>
+      </c>
+      <c r="N24">
+        <v>-13.561999999999999</v>
+      </c>
+      <c r="O24">
+        <f>N24/$C$12</f>
+        <v>-1.8219678650115535E-5</v>
+      </c>
+      <c r="Q24">
+        <v>4.3449999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>1.3816446343167286</v>
+      </c>
+      <c r="N25">
+        <v>0.31969999999999998</v>
+      </c>
+      <c r="O25">
+        <f>N25/$C$12</f>
+        <v>4.2949648019775373E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>1.5277133257258779</v>
+      </c>
+      <c r="N26">
+        <v>-2E-3</v>
+      </c>
+      <c r="O26">
+        <f>N26/$C$12</f>
+        <v>-2.6868719436831642E-9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>46</v>
+      </c>
+      <c r="B27">
+        <v>1.938101187597399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>2.2317574829383631</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>57</v>
+      </c>
+      <c r="B29">
+        <v>2.6737225814631671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30">
+        <v>63</v>
+      </c>
+      <c r="B30">
+        <v>2.9268875275404374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>